<commit_message>
barely working finite element method chamber thermal analysis
</commit_message>
<xml_diff>
--- a/mcnugget/propulsion/cta/fem/input_sheets/cta_fem_input_0.xlsx
+++ b/mcnugget/propulsion/cta/fem/input_sheets/cta_fem_input_0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate Campbell\Desktop\MASA2\mcnugget\mcnugget\propulsion\cta\fem\input_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9361325B-A34A-4C04-9C79-2C12825E5DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0160F8-1114-409B-B505-FA4AAA562812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>injector inlet pressure</t>
   </si>
@@ -86,9 +86,6 @@
     <t>nozzle length from throat</t>
   </si>
   <si>
-    <t>nozzle contour inputs</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -122,39 +119,21 @@
     <t>theta_i</t>
   </si>
   <si>
-    <t>percent length</t>
-  </si>
-  <si>
-    <t>L_p</t>
-  </si>
-  <si>
-    <t>propellant inputs</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>RP-1</t>
   </si>
   <si>
-    <t>combustion inputs</t>
-  </si>
-  <si>
     <t>combustion temperature</t>
   </si>
   <si>
-    <t>T_c</t>
-  </si>
-  <si>
     <t>chamber stagnation temperature</t>
   </si>
   <si>
     <t>p_inj</t>
   </si>
   <si>
-    <t>hot gas heat transfer inputs</t>
-  </si>
-  <si>
     <t>specific heat ratio</t>
   </si>
   <si>
@@ -167,9 +146,6 @@
     <t>mm</t>
   </si>
   <si>
-    <t>cooling channel geometry inputs</t>
-  </si>
-  <si>
     <t>number of fins</t>
   </si>
   <si>
@@ -185,24 +161,82 @@
     <t>t_liner</t>
   </si>
   <si>
-    <t>w_fin</t>
-  </si>
-  <si>
     <t>n_fin</t>
   </si>
   <si>
-    <t>width of fins</t>
-  </si>
-  <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>number of stations</t>
+  </si>
+  <si>
+    <t>Nc</t>
+  </si>
+  <si>
+    <t>ambient heat transfer</t>
+  </si>
+  <si>
+    <t>hot gas heat transfer</t>
+  </si>
+  <si>
+    <t>combustion</t>
+  </si>
+  <si>
+    <t>cooling channel geometry</t>
+  </si>
+  <si>
+    <t>nozzle contour</t>
+  </si>
+  <si>
+    <t>propellant</t>
+  </si>
+  <si>
+    <t>ambient air temperature</t>
+  </si>
+  <si>
+    <t>T_amb</t>
+  </si>
+  <si>
+    <t>ambient convection coefficient</t>
+  </si>
+  <si>
+    <t>h_amb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel inlet location </t>
+  </si>
+  <si>
+    <t>x_fuel_in</t>
+  </si>
+  <si>
+    <t>width of channels</t>
+  </si>
+  <si>
+    <t>w_cc</t>
+  </si>
+  <si>
+    <t>jacket wall thickness</t>
+  </si>
+  <si>
+    <t>t_j</t>
+  </si>
+  <si>
+    <t>initial fuel temperature</t>
+  </si>
+  <si>
+    <t>T_init_f</t>
+  </si>
+  <si>
+    <t>T0g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -241,11 +275,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E30"/>
+  <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -545,18 +580,18 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -588,120 +623,120 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
         <v>0.127</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>7.6200000000000004E-2</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7">
-        <v>0.15240000000000001</v>
+        <v>7.6200000000000004E-2</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.52359877559829882</v>
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>0.15240000000000001</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
-        <v>0.254</v>
+        <v>23</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.52359877559829882</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10">
-        <v>1.2</v>
+        <v>0.254</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11">
-        <v>0.35</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.4014257279586958</v>
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>0.35</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2">
-        <v>0.23561944901923448</v>
+        <v>0.4014257279586958</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14">
-        <v>0.8</v>
+        <v>24</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.23561944901923448</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.55000000000000004">
@@ -709,7 +744,7 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2">
         <v>0.11515737745896172</v>
@@ -717,112 +752,167 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
       <c r="D16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16">
+        <v>44</v>
+      </c>
+      <c r="E16" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17">
         <f>CONVERT(0.1,"in","m")</f>
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-    </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
         <f>CONVERT(0.04,"in","m")</f>
         <v>1.016E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20">
         <f>CONVERT(0.1,"in","m")</f>
         <v>2.5400000000000002E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20">
-        <v>3300</v>
-      </c>
-    </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="3">
+        <v>56</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.36915737745896171</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="2">
+        <f>CONVERT(0.1,"in","m")</f>
+        <v>2.5400000000000002E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="4">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3">
         <f>CONVERT(300,"psi","Pa")</f>
         <v>2068427.1879505084</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
         <v>1.23</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>